<commit_message>
Clean up of in and out-put files
</commit_message>
<xml_diff>
--- a/model_parameters/Road_dust_parameter_table_example.xlsx
+++ b/model_parameters/Road_dust_parameter_table_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sindredenby/Documents/metrologisk/NORTRIP-python/model_parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prog\NORTRIP-python\model_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BB6D09-0E32-5A4C-8996-944B7BBBFDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178DB7ED-4A4A-41DE-A9B9-AFA53D94C38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="27060" windowHeight="14160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -4543,9 +4543,6 @@
     <t>Use the underlaying subsurface in the energy balance calculations. 1 using air temp, 2 using slab temp</t>
   </si>
   <si>
-    <t>Set to 0 if no speed dependence required. Default is 0.012</t>
-  </si>
-  <si>
     <t>Default was 10</t>
   </si>
   <si>
@@ -4649,6 +4646,9 @@
   </si>
   <si>
     <t>1 is normal forecast, 2 is persistence, 3 is bias correction from last obs, 4 is interpolated trend (last two measurements) bias correction</t>
+  </si>
+  <si>
+    <t>Set to 0 if no speed dependence required. Default was originally 0.012</t>
   </si>
 </sst>
 </file>
@@ -5976,27 +5976,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" zoomScale="180" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A148" sqref="A148"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.5" customWidth="1"/>
-    <col min="2" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="6" width="20.1640625" customWidth="1"/>
-    <col min="7" max="7" width="54.6640625" style="86" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" customWidth="1"/>
+    <col min="2" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="54.7109375" style="86" customWidth="1"/>
     <col min="8" max="8" width="19" style="6" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="6" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="6" customWidth="1"/>
     <col min="11" max="11" width="16" style="6" customWidth="1"/>
     <col min="12" max="12" width="21" style="6" customWidth="1"/>
-    <col min="13" max="13" width="14.5" style="6" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.1640625" style="6"/>
+    <col min="13" max="13" width="14.42578125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>17</v>
       </c>
@@ -6019,14 +6019,14 @@
         <v>281</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E2" s="69"/>
       <c r="F2" s="69"/>
       <c r="G2" s="77" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>133</v>
       </c>
@@ -6051,7 +6051,7 @@
       <c r="N3" s="96"/>
       <c r="P3" s="6"/>
     </row>
-    <row r="4" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -6081,7 +6081,7 @@
       </c>
       <c r="N4" s="97"/>
     </row>
-    <row r="5" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>83</v>
       </c>
@@ -6119,7 +6119,7 @@
       </c>
       <c r="N5" s="98"/>
     </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>87</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
         <v>88</v>
       </c>
@@ -6186,7 +6186,7 @@
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="64" t="s">
         <v>244</v>
       </c>
@@ -6211,7 +6211,7 @@
       <c r="J8" s="29"/>
       <c r="K8" s="30"/>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="64" t="s">
         <v>399</v>
       </c>
@@ -6236,7 +6236,7 @@
       <c r="J9" s="29"/>
       <c r="K9" s="30"/>
     </row>
-    <row r="10" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>82</v>
       </c>
@@ -6247,7 +6247,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="78"/>
     </row>
-    <row r="11" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>89</v>
       </c>
@@ -6267,7 +6267,7 @@
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -6287,7 +6287,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="78"/>
     </row>
-    <row r="13" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="s">
         <v>2</v>
       </c>
@@ -6304,7 +6304,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="78"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="64" t="s">
         <v>244</v>
       </c>
@@ -6329,7 +6329,7 @@
       <c r="J14" s="29"/>
       <c r="K14" s="30"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="64" t="s">
         <v>399</v>
       </c>
@@ -6354,7 +6354,7 @@
       <c r="J15" s="29"/>
       <c r="K15" s="30"/>
     </row>
-    <row r="16" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>90</v>
       </c>
@@ -6394,13 +6394,13 @@
         <v>1</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J17" s="10">
         <v>1.9</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>1</v>
       </c>
@@ -6423,13 +6423,13 @@
         <v>2</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J18" s="10">
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
         <v>2</v>
       </c>
@@ -6449,13 +6449,13 @@
         <v>3</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J19" s="10">
         <v>2.9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="64" t="s">
         <v>244</v>
       </c>
@@ -6479,14 +6479,14 @@
         <v>4</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J20" s="10">
         <v>3.6</v>
       </c>
       <c r="K20" s="30"/>
     </row>
-    <row r="21" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="64" t="s">
         <v>399</v>
       </c>
@@ -6510,14 +6510,14 @@
         <v>5</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J21" s="10">
         <v>1.5</v>
       </c>
       <c r="K21" s="29"/>
     </row>
-    <row r="22" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>64</v>
       </c>
@@ -6531,13 +6531,13 @@
         <v>6</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J22" s="10">
         <v>1.98</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>14</v>
       </c>
@@ -6553,13 +6553,13 @@
         <v>7</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J23" s="10">
         <v>2.56</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>91</v>
       </c>
@@ -6577,13 +6577,13 @@
         <v>8</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J24" s="10">
         <v>3.28</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>4</v>
       </c>
@@ -6597,13 +6597,13 @@
         <v>9</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J25" s="10">
         <v>2.1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>131</v>
       </c>
@@ -6621,13 +6621,13 @@
         <v>10</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J26" s="10">
         <v>2.5299999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>92</v>
       </c>
@@ -6647,21 +6647,21 @@
         <v>11</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J27" s="10">
         <v>3.11</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>1</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C28" s="10">
-        <v>1</v>
+        <v>3.6</v>
       </c>
       <c r="D28" s="10">
         <v>1</v>
@@ -6673,18 +6673,18 @@
         <v>12</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J28" s="10">
         <v>3.83</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <v>2</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C29" s="10">
         <v>2.9</v>
@@ -6696,12 +6696,12 @@
       <c r="H29" s="30"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>3</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C30" s="10">
         <v>2.3199999999999998</v>
@@ -6711,16 +6711,16 @@
       <c r="F30" s="6"/>
       <c r="G30" s="78"/>
       <c r="H30" s="30" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <v>4</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C31" s="10">
         <v>1.9</v>
@@ -6732,7 +6732,7 @@
       <c r="H31" s="30"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
         <v>5</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <v>6</v>
       </c>
@@ -6781,7 +6781,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <v>7</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9">
         <v>8</v>
       </c>
@@ -6829,7 +6829,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9">
         <v>9</v>
       </c>
@@ -6854,12 +6854,12 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9">
         <v>10</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C37" s="10">
         <v>0.98</v>
@@ -6880,7 +6880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>7</v>
       </c>
@@ -6900,7 +6900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>132</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>94</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9">
         <v>1</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9">
         <v>2</v>
       </c>
@@ -6994,7 +6994,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9">
         <v>3</v>
       </c>
@@ -7009,7 +7009,7 @@
       <c r="F43" s="6"/>
       <c r="G43" s="78"/>
     </row>
-    <row r="44" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
         <v>4</v>
       </c>
@@ -7024,7 +7024,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="78"/>
     </row>
-    <row r="45" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>11</v>
       </c>
@@ -7035,7 +7035,7 @@
       <c r="F45" s="6"/>
       <c r="G45" s="78"/>
     </row>
-    <row r="46" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>96</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>1</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="28" t="s">
         <v>2</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="64" t="s">
         <v>244</v>
       </c>
@@ -7140,7 +7140,7 @@
       <c r="J49" s="29"/>
       <c r="K49" s="30"/>
     </row>
-    <row r="50" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="64" t="s">
         <v>400</v>
       </c>
@@ -7165,7 +7165,7 @@
       <c r="J50" s="29"/>
       <c r="K50" s="30"/>
     </row>
-    <row r="51" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>257</v>
       </c>
@@ -7176,7 +7176,7 @@
       <c r="F51" s="6"/>
       <c r="G51" s="78"/>
     </row>
-    <row r="52" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>256</v>
       </c>
@@ -7195,7 +7195,7 @@
       <c r="F52" s="58"/>
       <c r="G52" s="79"/>
     </row>
-    <row r="53" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="13" t="s">
         <v>249</v>
       </c>
@@ -7217,7 +7217,7 @@
       <c r="K53" s="20"/>
       <c r="L53" s="20"/>
     </row>
-    <row r="54" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="13" t="s">
         <v>250</v>
       </c>
@@ -7239,7 +7239,7 @@
       <c r="K54" s="20"/>
       <c r="L54" s="20"/>
     </row>
-    <row r="55" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="42" t="s">
         <v>251</v>
       </c>
@@ -7261,7 +7261,7 @@
       <c r="K55" s="20"/>
       <c r="L55" s="20"/>
     </row>
-    <row r="56" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="44" t="s">
         <v>252</v>
       </c>
@@ -7283,7 +7283,7 @@
       <c r="K56" s="20"/>
       <c r="L56" s="20"/>
     </row>
-    <row r="57" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="13" t="s">
         <v>254</v>
       </c>
@@ -7305,7 +7305,7 @@
       <c r="K57" s="20"/>
       <c r="L57" s="20"/>
     </row>
-    <row r="58" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="13" t="s">
         <v>255</v>
       </c>
@@ -7327,7 +7327,7 @@
       <c r="K58" s="20"/>
       <c r="L58" s="20"/>
     </row>
-    <row r="59" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="13" t="s">
         <v>253</v>
       </c>
@@ -7349,7 +7349,7 @@
       <c r="K59" s="20"/>
       <c r="L59" s="20"/>
     </row>
-    <row r="60" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="13" t="s">
         <v>258</v>
       </c>
@@ -7371,7 +7371,7 @@
       <c r="K60" s="20"/>
       <c r="L60" s="20"/>
     </row>
-    <row r="61" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
         <v>259</v>
       </c>
@@ -7393,7 +7393,7 @@
       <c r="K61" s="20"/>
       <c r="L61" s="20"/>
     </row>
-    <row r="62" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="13" t="s">
         <v>340</v>
       </c>
@@ -7417,7 +7417,7 @@
       <c r="K62" s="20"/>
       <c r="L62" s="20"/>
     </row>
-    <row r="63" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>297</v>
       </c>
@@ -7430,7 +7430,7 @@
       <c r="K63" s="20"/>
       <c r="L63" s="20"/>
     </row>
-    <row r="64" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>298</v>
       </c>
@@ -7449,7 +7449,7 @@
       <c r="K64" s="20"/>
       <c r="L64" s="20"/>
     </row>
-    <row r="65" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
         <v>1</v>
       </c>
@@ -7468,12 +7468,12 @@
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
       <c r="G65" s="78" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K65" s="20"/>
       <c r="L65" s="20"/>
     </row>
-    <row r="66" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="28" t="s">
         <v>2</v>
       </c>
@@ -7495,7 +7495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="41" t="s">
         <v>301</v>
       </c>
@@ -7512,7 +7512,7 @@
       <c r="J67" s="29"/>
       <c r="K67" s="30"/>
     </row>
-    <row r="68" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
         <v>299</v>
       </c>
@@ -7531,7 +7531,7 @@
       <c r="F68" s="58"/>
       <c r="G68" s="79"/>
     </row>
-    <row r="69" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="13" t="s">
         <v>302</v>
       </c>
@@ -7555,7 +7555,7 @@
       <c r="K69" s="20"/>
       <c r="L69" s="20"/>
     </row>
-    <row r="70" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>60</v>
       </c>
@@ -7566,7 +7566,7 @@
       <c r="F70" s="6"/>
       <c r="G70" s="78"/>
     </row>
-    <row r="71" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>97</v>
       </c>
@@ -7582,10 +7582,10 @@
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
       <c r="G71" s="78" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
         <v>1</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="28" t="s">
         <v>2</v>
       </c>
@@ -7629,7 +7629,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="41" t="s">
         <v>117</v>
       </c>
@@ -7646,7 +7646,7 @@
       <c r="J74" s="29"/>
       <c r="K74" s="30"/>
     </row>
-    <row r="75" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
         <v>282</v>
       </c>
@@ -7665,7 +7665,7 @@
       <c r="F75" s="58"/>
       <c r="G75" s="79"/>
     </row>
-    <row r="76" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="13" t="s">
         <v>283</v>
       </c>
@@ -7689,7 +7689,7 @@
       <c r="K76" s="20"/>
       <c r="L76" s="20"/>
     </row>
-    <row r="77" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>286</v>
       </c>
@@ -7700,7 +7700,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="78"/>
     </row>
-    <row r="78" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="12" t="s">
         <v>256</v>
       </c>
@@ -7716,7 +7716,7 @@
       <c r="G78" s="78"/>
       <c r="O78"/>
     </row>
-    <row r="79" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
         <v>287</v>
       </c>
@@ -7732,7 +7732,7 @@
       <c r="G79" s="78"/>
       <c r="O79"/>
     </row>
-    <row r="80" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="13" t="s">
         <v>288</v>
       </c>
@@ -7748,7 +7748,7 @@
       <c r="G80" s="78"/>
       <c r="O80"/>
     </row>
-    <row r="81" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="42" t="s">
         <v>289</v>
       </c>
@@ -7764,7 +7764,7 @@
       <c r="G81" s="78"/>
       <c r="O81"/>
     </row>
-    <row r="82" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="44" t="s">
         <v>290</v>
       </c>
@@ -7780,7 +7780,7 @@
       <c r="G82" s="78"/>
       <c r="O82"/>
     </row>
-    <row r="83" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="13" t="s">
         <v>291</v>
       </c>
@@ -7796,7 +7796,7 @@
       <c r="G83" s="78"/>
       <c r="O83"/>
     </row>
-    <row r="84" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="13" t="s">
         <v>292</v>
       </c>
@@ -7812,7 +7812,7 @@
       <c r="G84" s="78"/>
       <c r="O84"/>
     </row>
-    <row r="85" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="13" t="s">
         <v>293</v>
       </c>
@@ -7827,7 +7827,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="78"/>
     </row>
-    <row r="86" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="13" t="s">
         <v>294</v>
       </c>
@@ -7843,7 +7843,7 @@
       <c r="G86" s="78"/>
       <c r="P86" s="6"/>
     </row>
-    <row r="87" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="13" t="s">
         <v>295</v>
       </c>
@@ -7862,7 +7862,7 @@
       <c r="K87" s="20"/>
       <c r="P87" s="6"/>
     </row>
-    <row r="88" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>12</v>
       </c>
@@ -7877,7 +7877,7 @@
       <c r="K88" s="20"/>
       <c r="P88" s="6"/>
     </row>
-    <row r="89" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
         <v>276</v>
       </c>
@@ -7894,7 +7894,7 @@
       <c r="K89" s="20"/>
       <c r="P89" s="6"/>
     </row>
-    <row r="90" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="13" t="s">
         <v>98</v>
       </c>
@@ -7911,7 +7911,7 @@
       <c r="K90" s="20"/>
       <c r="P90" s="6"/>
     </row>
-    <row r="91" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="13" t="s">
         <v>277</v>
       </c>
@@ -7928,7 +7928,7 @@
       <c r="K91" s="20"/>
       <c r="P91" s="6"/>
     </row>
-    <row r="92" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="13" t="s">
         <v>99</v>
       </c>
@@ -7945,7 +7945,7 @@
       <c r="K92" s="20"/>
       <c r="P92" s="6"/>
     </row>
-    <row r="93" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="13" t="s">
         <v>100</v>
       </c>
@@ -7962,7 +7962,7 @@
       <c r="K93" s="20"/>
       <c r="P93" s="6"/>
     </row>
-    <row r="94" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="13" t="s">
         <v>300</v>
       </c>
@@ -7979,7 +7979,7 @@
       <c r="K94" s="20"/>
       <c r="P94" s="6"/>
     </row>
-    <row r="95" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="13" t="s">
         <v>275</v>
       </c>
@@ -7998,7 +7998,7 @@
       <c r="K95" s="20"/>
       <c r="P95" s="6"/>
     </row>
-    <row r="96" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>346</v>
       </c>
@@ -8013,7 +8013,7 @@
       <c r="J96" s="29"/>
       <c r="K96" s="30"/>
     </row>
-    <row r="97" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
         <v>256</v>
       </c>
@@ -8036,7 +8036,7 @@
       <c r="J97" s="29"/>
       <c r="K97" s="30"/>
     </row>
-    <row r="98" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="13" t="s">
         <v>233</v>
       </c>
@@ -8057,7 +8057,7 @@
       <c r="F98" s="20"/>
       <c r="G98" s="81"/>
     </row>
-    <row r="99" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="13" t="s">
         <v>234</v>
       </c>
@@ -8075,12 +8075,12 @@
       </c>
       <c r="F99" s="20"/>
       <c r="G99" s="81" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="L99" s="20"/>
       <c r="M99" s="20"/>
     </row>
-    <row r="100" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="42" t="s">
         <v>235</v>
       </c>
@@ -8102,7 +8102,7 @@
       <c r="L100" s="20"/>
       <c r="M100" s="20"/>
     </row>
-    <row r="101" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="44" t="s">
         <v>236</v>
       </c>
@@ -8111,24 +8111,24 @@
       </c>
       <c r="C101" s="10">
         <f>0.05*G101</f>
-        <v>0.05</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D101" s="114">
         <f>C101*0.16</f>
-        <v>8.0000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E101" s="10">
         <f>C101*0.04</f>
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="F101" s="20"/>
       <c r="G101" s="81">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L101" s="20"/>
       <c r="M101" s="20"/>
     </row>
-    <row r="102" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="13" t="s">
         <v>241</v>
       </c>
@@ -8150,7 +8150,7 @@
       <c r="L102" s="20"/>
       <c r="M102" s="20"/>
     </row>
-    <row r="103" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="13" t="s">
         <v>242</v>
       </c>
@@ -8176,7 +8176,7 @@
       <c r="M103" s="20"/>
       <c r="O103"/>
     </row>
-    <row r="104" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="13" t="s">
         <v>237</v>
       </c>
@@ -8201,7 +8201,7 @@
       <c r="L104" s="20"/>
       <c r="O104"/>
     </row>
-    <row r="105" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="13" t="s">
         <v>239</v>
       </c>
@@ -8229,7 +8229,7 @@
       <c r="L105" s="20"/>
       <c r="O105"/>
     </row>
-    <row r="106" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="13" t="s">
         <v>240</v>
       </c>
@@ -8258,7 +8258,7 @@
       <c r="M106" s="20"/>
       <c r="O106"/>
     </row>
-    <row r="107" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="13" t="s">
         <v>306</v>
       </c>
@@ -8286,7 +8286,7 @@
       <c r="M107" s="20"/>
       <c r="O107"/>
     </row>
-    <row r="108" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="13" t="s">
         <v>307</v>
       </c>
@@ -8315,7 +8315,7 @@
       <c r="M108" s="20"/>
       <c r="O108"/>
     </row>
-    <row r="109" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="41" t="s">
         <v>118</v>
       </c>
@@ -8334,7 +8334,7 @@
       <c r="L109" s="20"/>
       <c r="O109"/>
     </row>
-    <row r="110" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="41" t="s">
         <v>119</v>
       </c>
@@ -8345,10 +8345,10 @@
       <c r="E110" s="6"/>
       <c r="F110" s="6"/>
       <c r="G110" s="93" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>13</v>
       </c>
@@ -8362,7 +8362,7 @@
       <c r="K111" s="20"/>
       <c r="L111" s="20"/>
     </row>
-    <row r="112" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="12" t="s">
         <v>14</v>
       </c>
@@ -8378,7 +8378,7 @@
       <c r="K112" s="20"/>
       <c r="L112" s="20"/>
     </row>
-    <row r="113" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="18" t="s">
         <v>103</v>
       </c>
@@ -8394,7 +8394,7 @@
       <c r="K113" s="20"/>
       <c r="L113" s="20"/>
     </row>
-    <row r="114" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="13" t="s">
         <v>104</v>
       </c>
@@ -8410,7 +8410,7 @@
       <c r="K114" s="20"/>
       <c r="L114" s="20"/>
     </row>
-    <row r="115" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>61</v>
       </c>
@@ -8421,7 +8421,7 @@
       <c r="F115" s="6"/>
       <c r="G115" s="79"/>
     </row>
-    <row r="116" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="12" t="s">
         <v>263</v>
       </c>
@@ -8440,7 +8440,7 @@
       <c r="F116" s="58"/>
       <c r="G116" s="81"/>
     </row>
-    <row r="117" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="13" t="s">
         <v>105</v>
       </c>
@@ -8462,7 +8462,7 @@
       <c r="F117" s="20"/>
       <c r="G117" s="81"/>
     </row>
-    <row r="118" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="13" t="s">
         <v>106</v>
       </c>
@@ -8481,7 +8481,7 @@
       <c r="F118" s="20"/>
       <c r="G118" s="81"/>
     </row>
-    <row r="119" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="13" t="s">
         <v>107</v>
       </c>
@@ -8506,7 +8506,7 @@
       <c r="L119" s="20"/>
       <c r="M119" s="20"/>
     </row>
-    <row r="120" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="13" t="s">
         <v>108</v>
       </c>
@@ -8534,7 +8534,7 @@
       <c r="L120" s="20"/>
       <c r="M120" s="20"/>
     </row>
-    <row r="121" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="12" t="s">
         <v>264</v>
       </c>
@@ -8551,7 +8551,7 @@
       <c r="L121" s="20"/>
       <c r="M121" s="20"/>
     </row>
-    <row r="122" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="13" t="s">
         <v>105</v>
       </c>
@@ -8566,7 +8566,7 @@
       <c r="F122" s="20"/>
       <c r="G122" s="81"/>
     </row>
-    <row r="123" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="13" t="s">
         <v>106</v>
       </c>
@@ -8589,7 +8589,7 @@
       <c r="N123" s="6"/>
       <c r="O123" s="6"/>
     </row>
-    <row r="124" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="13" t="s">
         <v>107</v>
       </c>
@@ -8612,7 +8612,7 @@
       <c r="N124" s="6"/>
       <c r="O124" s="6"/>
     </row>
-    <row r="125" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="13" t="s">
         <v>108</v>
       </c>
@@ -8635,7 +8635,7 @@
       <c r="N125" s="6"/>
       <c r="O125" s="6"/>
     </row>
-    <row r="126" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>16</v>
       </c>
@@ -8654,7 +8654,7 @@
       <c r="N126" s="6"/>
       <c r="O126" s="6"/>
     </row>
-    <row r="127" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="8"/>
       <c r="B127" s="8" t="s">
         <v>280</v>
@@ -8677,7 +8677,7 @@
       <c r="N127" s="6"/>
       <c r="O127" s="6"/>
     </row>
-    <row r="128" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="13" t="s">
         <v>109</v>
       </c>
@@ -8702,7 +8702,7 @@
       <c r="N128" s="6"/>
       <c r="O128" s="6"/>
     </row>
-    <row r="129" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>135</v>
       </c>
@@ -8717,7 +8717,7 @@
       <c r="J129" s="29"/>
       <c r="K129" s="30"/>
     </row>
-    <row r="130" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
         <v>14</v>
       </c>
@@ -8738,7 +8738,7 @@
       <c r="N130" s="6"/>
       <c r="O130" s="6"/>
     </row>
-    <row r="131" spans="1:15" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="18" t="s">
         <v>136</v>
       </c>
@@ -8761,7 +8761,7 @@
       <c r="N131" s="6"/>
       <c r="O131" s="6"/>
     </row>
-    <row r="132" spans="1:15" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="13" t="s">
         <v>137</v>
       </c>
@@ -8784,7 +8784,7 @@
       <c r="N132" s="6"/>
       <c r="O132" s="6"/>
     </row>
-    <row r="133" spans="1:15" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:15" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="19"/>
       <c r="B133" s="20"/>
       <c r="C133" s="20"/>
@@ -8820,7 +8820,7 @@
       <c r="N134" s="6"/>
       <c r="O134" s="6"/>
     </row>
-    <row r="135" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>18</v>
       </c>
@@ -8839,7 +8839,7 @@
       <c r="N135" s="6"/>
       <c r="O135" s="6"/>
     </row>
-    <row r="136" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
         <v>14</v>
       </c>
@@ -8864,7 +8864,7 @@
       <c r="N136" s="6"/>
       <c r="O136" s="6"/>
     </row>
-    <row r="137" spans="1:15" s="2" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" s="2" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="13" t="s">
         <v>337</v>
       </c>
@@ -8892,7 +8892,7 @@
       <c r="N137" s="6"/>
       <c r="O137" s="6"/>
     </row>
-    <row r="138" spans="1:15" s="2" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" s="2" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="13" t="s">
         <v>338</v>
       </c>
@@ -8930,7 +8930,7 @@
       <c r="N138" s="6"/>
       <c r="O138" s="6"/>
     </row>
-    <row r="139" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="13" t="s">
         <v>111</v>
       </c>
@@ -8955,7 +8955,7 @@
       <c r="N139" s="6"/>
       <c r="O139" s="6"/>
     </row>
-    <row r="140" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="13" t="s">
         <v>112</v>
       </c>
@@ -8980,7 +8980,7 @@
       <c r="N140" s="6"/>
       <c r="O140" s="6"/>
     </row>
-    <row r="141" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="41" t="s">
         <v>228</v>
       </c>
@@ -9007,7 +9007,7 @@
       <c r="N141" s="6"/>
       <c r="O141" s="6"/>
     </row>
-    <row r="142" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="13" t="s">
         <v>229</v>
       </c>
@@ -9032,7 +9032,7 @@
       <c r="N142" s="6"/>
       <c r="O142" s="6"/>
     </row>
-    <row r="143" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>44</v>
       </c>
@@ -9051,7 +9051,7 @@
       <c r="N143" s="6"/>
       <c r="O143" s="6"/>
     </row>
-    <row r="144" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A144" s="43" t="s">
         <v>14</v>
       </c>
@@ -9075,7 +9075,7 @@
       <c r="N144" s="6"/>
       <c r="O144" s="6"/>
     </row>
-    <row r="145" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="44" t="s">
         <v>113</v>
       </c>
@@ -9101,7 +9101,7 @@
       <c r="N145" s="6"/>
       <c r="O145" s="6"/>
     </row>
-    <row r="146" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A146" s="44" t="s">
         <v>196</v>
       </c>
@@ -9121,7 +9121,7 @@
       <c r="N146" s="6"/>
       <c r="O146" s="6"/>
     </row>
-    <row r="147" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A147" s="44" t="s">
         <v>351</v>
       </c>
@@ -9141,7 +9141,7 @@
       <c r="N147" s="6"/>
       <c r="O147" s="6"/>
     </row>
-    <row r="148" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>20</v>
       </c>
@@ -9160,7 +9160,7 @@
       <c r="N148" s="6"/>
       <c r="O148" s="6"/>
     </row>
-    <row r="149" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
         <v>14</v>
       </c>
@@ -9185,7 +9185,7 @@
       <c r="N149" s="6"/>
       <c r="O149" s="6"/>
     </row>
-    <row r="150" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A150" s="13" t="s">
         <v>120</v>
       </c>
@@ -9212,7 +9212,7 @@
       <c r="N150" s="6"/>
       <c r="O150" s="6"/>
     </row>
-    <row r="151" spans="1:15" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
         <v>21</v>
       </c>
@@ -9254,7 +9254,7 @@
       <c r="N152" s="39"/>
       <c r="O152" s="39"/>
     </row>
-    <row r="153" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="12" t="s">
         <v>14</v>
       </c>
@@ -9267,7 +9267,7 @@
       <c r="F153" s="6"/>
       <c r="G153" s="78"/>
     </row>
-    <row r="154" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="13" t="s">
         <v>114</v>
       </c>
@@ -9280,7 +9280,7 @@
       <c r="F154" s="6"/>
       <c r="G154" s="78"/>
     </row>
-    <row r="155" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="13" t="s">
         <v>74</v>
       </c>
@@ -9297,7 +9297,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="13" t="s">
         <v>68</v>
       </c>
@@ -9312,7 +9312,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="13" t="s">
         <v>123</v>
       </c>
@@ -9324,7 +9324,7 @@
       <c r="F157" s="6"/>
       <c r="G157" s="78"/>
     </row>
-    <row r="158" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="13" t="s">
         <v>356</v>
       </c>
@@ -9336,7 +9336,7 @@
       <c r="F158" s="6"/>
       <c r="G158" s="78"/>
     </row>
-    <row r="159" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="13" t="s">
         <v>122</v>
       </c>
@@ -9361,7 +9361,7 @@
       </c>
       <c r="J159" s="61"/>
     </row>
-    <row r="160" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="13" t="s">
         <v>122</v>
       </c>
@@ -9386,7 +9386,7 @@
       </c>
       <c r="J160"/>
     </row>
-    <row r="161" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="12" t="s">
         <v>125</v>
       </c>
@@ -9401,7 +9401,7 @@
       <c r="F161" s="6"/>
       <c r="G161" s="78"/>
     </row>
-    <row r="162" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="13" t="s">
         <v>121</v>
       </c>
@@ -9417,7 +9417,7 @@
       <c r="F162" s="6"/>
       <c r="G162" s="78"/>
     </row>
-    <row r="163" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A163" s="13" t="s">
         <v>124</v>
       </c>
@@ -9432,13 +9432,13 @@
       <c r="E163" s="6"/>
       <c r="F163" s="6"/>
       <c r="G163" s="84" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H163" s="21">
         <v>50</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>23</v>
       </c>
@@ -9449,7 +9449,7 @@
       <c r="F164" s="39"/>
       <c r="G164" s="85"/>
     </row>
-    <row r="165" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="12" t="s">
         <v>14</v>
       </c>
@@ -9475,12 +9475,12 @@
         <v>232</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="13" t="s">
         <v>115</v>
       </c>
       <c r="B166" s="10">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="C166" s="10">
         <v>0.5</v>
@@ -9500,16 +9500,16 @@
       </c>
       <c r="K166" s="95"/>
     </row>
-    <row r="167" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B167" s="22">
-        <f>0.02</f>
-        <v>0.02</v>
+        <f>0.01</f>
+        <v>0.01</v>
       </c>
       <c r="C167" s="22">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D167" s="91">
         <v>50</v>
@@ -9527,9 +9527,9 @@
       </c>
       <c r="K167" s="95"/>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B168" s="20"/>
       <c r="C168" s="20"/>
@@ -9539,9 +9539,9 @@
       <c r="J168"/>
       <c r="K168" s="95"/>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" s="19" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B169" s="20">
         <v>0.4</v>
@@ -9580,13 +9580,13 @@
       <c r="N170" s="6"/>
       <c r="O170" s="6"/>
     </row>
-    <row r="171" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>313</v>
       </c>
       <c r="G171" s="78"/>
     </row>
-    <row r="172" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="12" t="s">
         <v>316</v>
       </c>
@@ -9598,7 +9598,7 @@
       </c>
       <c r="G172" s="78"/>
     </row>
-    <row r="173" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="44" t="s">
         <v>113</v>
       </c>
@@ -9611,7 +9611,7 @@
       </c>
       <c r="G173" s="78"/>
     </row>
-    <row r="174" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="7" t="s">
         <v>96</v>
       </c>
@@ -9621,7 +9621,7 @@
       </c>
       <c r="G174" s="78"/>
     </row>
-    <row r="175" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A175" s="13" t="s">
         <v>110</v>
       </c>
@@ -9631,7 +9631,7 @@
       </c>
       <c r="G175" s="78"/>
     </row>
-    <row r="176" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A176" s="13" t="s">
         <v>314</v>
       </c>
@@ -9641,7 +9641,7 @@
       </c>
       <c r="G176" s="78"/>
     </row>
-    <row r="177" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="13" t="s">
         <v>315</v>
       </c>
@@ -9651,13 +9651,13 @@
       </c>
       <c r="G177" s="78"/>
     </row>
-    <row r="178" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>325</v>
       </c>
       <c r="G178" s="78"/>
     </row>
-    <row r="179" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="12" t="s">
         <v>328</v>
       </c>
@@ -9676,7 +9676,7 @@
       <c r="F179" s="58"/>
       <c r="G179" s="79"/>
     </row>
-    <row r="180" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A180" s="13" t="s">
         <v>333</v>
       </c>
@@ -9698,7 +9698,7 @@
       <c r="K180" s="20"/>
       <c r="L180" s="20"/>
     </row>
-    <row r="181" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="13" t="s">
         <v>332</v>
       </c>
@@ -9720,7 +9720,7 @@
       <c r="K181" s="20"/>
       <c r="L181" s="20"/>
     </row>
-    <row r="182" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="13" t="s">
         <v>331</v>
       </c>
@@ -9742,7 +9742,7 @@
       <c r="K182" s="20"/>
       <c r="L182" s="20"/>
     </row>
-    <row r="183" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A183" s="13" t="s">
         <v>330</v>
       </c>
@@ -9764,7 +9764,7 @@
       <c r="K183" s="20"/>
       <c r="L183" s="20"/>
     </row>
-    <row r="184" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A184" s="13" t="s">
         <v>329</v>
       </c>
@@ -9786,7 +9786,7 @@
       <c r="K184" s="20"/>
       <c r="L184" s="20"/>
     </row>
-    <row r="185" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="12" t="s">
         <v>328</v>
       </c>
@@ -9805,7 +9805,7 @@
       <c r="F185" s="58"/>
       <c r="G185" s="79"/>
     </row>
-    <row r="186" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A186" s="13" t="s">
         <v>333</v>
       </c>
@@ -9827,7 +9827,7 @@
       <c r="K186" s="20"/>
       <c r="L186" s="20"/>
     </row>
-    <row r="187" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A187" s="13" t="s">
         <v>332</v>
       </c>
@@ -9849,7 +9849,7 @@
       <c r="K187" s="20"/>
       <c r="L187" s="20"/>
     </row>
-    <row r="188" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A188" s="13" t="s">
         <v>331</v>
       </c>
@@ -9871,7 +9871,7 @@
       <c r="K188" s="20"/>
       <c r="L188" s="20"/>
     </row>
-    <row r="189" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A189" s="13" t="s">
         <v>330</v>
       </c>
@@ -9893,7 +9893,7 @@
       <c r="K189" s="20"/>
       <c r="L189" s="20"/>
     </row>
-    <row r="190" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A190" s="13" t="s">
         <v>329</v>
       </c>
@@ -9924,22 +9924,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="181" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="79.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="79.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
         <v>56</v>
       </c>
@@ -9953,7 +9953,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
         <v>24</v>
       </c>
@@ -9967,7 +9967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="102" t="s">
         <v>183</v>
       </c>
@@ -9981,7 +9981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="102" t="s">
         <v>26</v>
       </c>
@@ -9995,7 +9995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="102" t="s">
         <v>310</v>
       </c>
@@ -10009,7 +10009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="102" t="s">
         <v>28</v>
       </c>
@@ -10023,7 +10023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="102" t="s">
         <v>194</v>
       </c>
@@ -10037,7 +10037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="102" t="s">
         <v>304</v>
       </c>
@@ -10051,7 +10051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="102" t="s">
         <v>63</v>
       </c>
@@ -10065,7 +10065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="102" t="s">
         <v>32</v>
       </c>
@@ -10079,7 +10079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="102" t="s">
         <v>45</v>
       </c>
@@ -10093,7 +10093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="102" t="s">
         <v>65</v>
       </c>
@@ -10107,7 +10107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="102" t="s">
         <v>30</v>
       </c>
@@ -10121,7 +10121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="99" t="s">
         <v>55</v>
       </c>
@@ -10129,7 +10129,7 @@
       <c r="C14" s="101"/>
       <c r="D14" s="100"/>
     </row>
-    <row r="15" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="102" t="s">
         <v>33</v>
       </c>
@@ -10143,7 +10143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="102" t="s">
         <v>34</v>
       </c>
@@ -10157,7 +10157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="102" t="s">
         <v>47</v>
       </c>
@@ -10171,7 +10171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="102" t="s">
         <v>353</v>
       </c>
@@ -10185,7 +10185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="102" t="s">
         <v>48</v>
       </c>
@@ -10199,7 +10199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="102" t="s">
         <v>67</v>
       </c>
@@ -10207,13 +10207,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="102" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D20" s="103">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="99" t="s">
         <v>129</v>
       </c>
@@ -10221,7 +10221,7 @@
       <c r="C21" s="101"/>
       <c r="D21" s="100"/>
     </row>
-    <row r="22" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="102" t="s">
         <v>35</v>
       </c>
@@ -10229,13 +10229,13 @@
         <v>2</v>
       </c>
       <c r="C22" s="102" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D22" s="103">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="102" t="s">
         <v>38</v>
       </c>
@@ -10249,7 +10249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="102" t="s">
         <v>40</v>
       </c>
@@ -10263,7 +10263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="102" t="s">
         <v>130</v>
       </c>
@@ -10277,7 +10277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="102" t="s">
         <v>203</v>
       </c>
@@ -10291,85 +10291,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="102" t="s">
+        <v>431</v>
+      </c>
+      <c r="B27" s="103">
+        <v>1</v>
+      </c>
+      <c r="C27" s="102" t="s">
         <v>432</v>
       </c>
-      <c r="B27" s="103">
-        <v>1</v>
-      </c>
-      <c r="C27" s="102" t="s">
-        <v>433</v>
-      </c>
       <c r="D27" s="103">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="99" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="100"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="102" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B29" s="103">
         <v>0</v>
       </c>
       <c r="C29" s="102" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D29" s="103">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="116" t="s">
+        <v>433</v>
+      </c>
+      <c r="B30" s="117">
+        <v>1</v>
+      </c>
+      <c r="C30" s="116" t="s">
         <v>434</v>
-      </c>
-      <c r="B30" s="117">
-        <v>1</v>
-      </c>
-      <c r="C30" s="116" t="s">
-        <v>435</v>
       </c>
       <c r="D30" s="117">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A31" s="102" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B31" s="103">
         <v>0</v>
       </c>
       <c r="C31" s="102" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D31" s="103">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A32" s="116" t="s">
+        <v>440</v>
+      </c>
+      <c r="B32" s="117">
+        <v>1</v>
+      </c>
+      <c r="C32" s="118" t="s">
         <v>441</v>
       </c>
-      <c r="B32" s="117">
-        <v>1</v>
-      </c>
-      <c r="C32" s="118" t="s">
-        <v>442</v>
-      </c>
       <c r="D32" s="117">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="99" t="s">
         <v>57</v>
       </c>
@@ -10377,7 +10377,7 @@
       <c r="C33" s="101"/>
       <c r="D33" s="100"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="102" t="s">
         <v>271</v>
       </c>
@@ -10391,7 +10391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="102" t="s">
         <v>272</v>
       </c>
@@ -10405,7 +10405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="102" t="s">
         <v>50</v>
       </c>
@@ -10419,7 +10419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="102" t="s">
         <v>51</v>
       </c>
@@ -10433,7 +10433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="102" t="s">
         <v>72</v>
       </c>
@@ -10446,11 +10446,8 @@
       <c r="D38" s="103">
         <v>1</v>
       </c>
-      <c r="E38">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="102" t="s">
         <v>52</v>
       </c>
@@ -10464,12 +10461,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="102" t="s">
         <v>41</v>
       </c>
       <c r="B40" s="103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="102" t="s">
         <v>393</v>
@@ -10478,7 +10475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="102" t="s">
         <v>388</v>
       </c>
@@ -10492,7 +10489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="102" t="s">
         <v>42</v>
       </c>
@@ -10506,7 +10503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="102" t="s">
         <v>43</v>
       </c>
@@ -10520,7 +10517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="102" t="s">
         <v>198</v>
       </c>
@@ -10534,7 +10531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="99" t="s">
         <v>59</v>
       </c>
@@ -10542,7 +10539,7 @@
       <c r="C45" s="101"/>
       <c r="D45" s="100"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="102" t="s">
         <v>36</v>
       </c>
@@ -10556,21 +10553,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="102" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B47" s="103">
         <v>0</v>
       </c>
       <c r="C47" s="102" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D47" s="103">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="102" t="s">
         <v>37</v>
       </c>
@@ -10584,7 +10581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="99" t="s">
         <v>210</v>
       </c>
@@ -10592,7 +10589,7 @@
       <c r="C49" s="101"/>
       <c r="D49" s="100"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="102" t="s">
         <v>211</v>
       </c>
@@ -10606,8 +10603,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10625,13 +10622,13 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="89.5" style="24" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.42578125" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="104" t="s">
         <v>180</v>
       </c>
@@ -10642,10 +10639,10 @@
         <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="107" t="s">
         <v>154</v>
       </c>
@@ -10656,7 +10653,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="109" t="s">
         <v>184</v>
       </c>
@@ -10669,7 +10666,7 @@
       <c r="D3" s="92"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
         <v>143</v>
       </c>
@@ -10682,7 +10679,7 @@
       <c r="D4" s="92"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="109" t="s">
         <v>142</v>
       </c>
@@ -10695,7 +10692,7 @@
       <c r="D5" s="92"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="109" t="s">
         <v>141</v>
       </c>
@@ -10708,7 +10705,7 @@
       <c r="D6" s="92"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="109" t="s">
         <v>151</v>
       </c>
@@ -10723,7 +10720,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="109" t="s">
         <v>152</v>
       </c>
@@ -10738,7 +10735,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="109" t="s">
         <v>172</v>
       </c>
@@ -10753,7 +10750,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="109" t="s">
         <v>153</v>
       </c>
@@ -10768,7 +10765,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="109" t="s">
         <v>140</v>
       </c>
@@ -10781,7 +10778,7 @@
       <c r="D11" s="92"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="109" t="s">
         <v>144</v>
       </c>
@@ -10794,7 +10791,7 @@
       <c r="D12" s="92"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="109" t="s">
         <v>145</v>
       </c>
@@ -10807,7 +10804,7 @@
       <c r="D13" s="92"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="109" t="s">
         <v>347</v>
       </c>
@@ -10820,12 +10817,12 @@
       <c r="D14" s="92"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="112"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="107" t="s">
         <v>155</v>
       </c>
@@ -10836,7 +10833,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="109" t="s">
         <v>185</v>
       </c>
@@ -10847,7 +10844,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="109" t="s">
         <v>156</v>
       </c>
@@ -10858,7 +10855,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="109" t="s">
         <v>157</v>
       </c>
@@ -10869,7 +10866,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="109" t="s">
         <v>158</v>
       </c>
@@ -10880,7 +10877,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="109" t="s">
         <v>160</v>
       </c>
@@ -10891,7 +10888,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="109" t="s">
         <v>161</v>
       </c>
@@ -10902,7 +10899,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="109" t="s">
         <v>171</v>
       </c>
@@ -10913,7 +10910,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="109" t="s">
         <v>162</v>
       </c>
@@ -10924,7 +10921,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="109" t="s">
         <v>159</v>
       </c>
@@ -10935,7 +10932,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="109" t="s">
         <v>163</v>
       </c>
@@ -10946,7 +10943,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="109" t="s">
         <v>164</v>
       </c>
@@ -10957,12 +10954,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="112"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="107" t="s">
         <v>193</v>
       </c>
@@ -10973,7 +10970,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="109" t="s">
         <v>216</v>
       </c>
@@ -10984,7 +10981,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="109" t="s">
         <v>215</v>
       </c>
@@ -10993,12 +10990,12 @@
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="112"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="107" t="s">
         <v>199</v>
       </c>
@@ -11009,7 +11006,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="109" t="s">
         <v>218</v>
       </c>
@@ -11021,7 +11018,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="109" t="s">
         <v>219</v>
       </c>
@@ -11032,7 +11029,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="109" t="s">
         <v>220</v>
       </c>
@@ -11043,7 +11040,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="109" t="s">
         <v>221</v>
       </c>
@@ -11054,7 +11051,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="109" t="s">
         <v>200</v>
       </c>
@@ -11065,7 +11062,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="109" t="s">
         <v>222</v>
       </c>
@@ -11076,7 +11073,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="109" t="s">
         <v>269</v>
       </c>
@@ -11087,12 +11084,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="112"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="107" t="s">
         <v>366</v>
       </c>
@@ -11103,7 +11100,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="109" t="s">
         <v>367</v>
       </c>
@@ -11116,7 +11113,7 @@
       <c r="D43" s="92"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="109" t="s">
         <v>368</v>
       </c>
@@ -11129,7 +11126,7 @@
       <c r="D44" s="92"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="109" t="s">
         <v>369</v>
       </c>
@@ -11142,7 +11139,7 @@
       <c r="D45" s="92"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="109" t="s">
         <v>370</v>
       </c>
@@ -11155,7 +11152,7 @@
       <c r="D46" s="92"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="109" t="s">
         <v>371</v>
       </c>
@@ -11168,7 +11165,7 @@
       <c r="D47" s="92"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="109" t="s">
         <v>372</v>
       </c>
@@ -11181,7 +11178,7 @@
       <c r="D48" s="92"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="109" t="s">
         <v>373</v>
       </c>
@@ -11194,7 +11191,7 @@
       <c r="D49" s="92"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="109" t="s">
         <v>374</v>
       </c>
@@ -11207,7 +11204,7 @@
       <c r="D50" s="92"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="109" t="s">
         <v>375</v>
       </c>
@@ -11220,7 +11217,7 @@
       <c r="D51" s="92"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="109" t="s">
         <v>376</v>
       </c>
@@ -11233,7 +11230,7 @@
       <c r="D52" s="92"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="109" t="s">
         <v>377</v>
       </c>
@@ -11246,7 +11243,7 @@
       <c r="D53" s="92"/>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="109" t="s">
         <v>378</v>
       </c>
@@ -11257,7 +11254,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="109" t="s">
         <v>379</v>
       </c>

</xml_diff>